<commit_message>
Updated file upload code in Appendices feature
Due to enhancement done on production, I have to change code for upload
files functionality.
</commit_message>
<xml_diff>
--- a/Parcel-Test-Features/Appendices/bin/Test_Data/Appendices.xlsx
+++ b/Parcel-Test-Features/Appendices/bin/Test_Data/Appendices.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Site ID" sheetId="2" r:id="rId1"/>
     <sheet name="Credentials" sheetId="3" r:id="rId2"/>
-    <sheet name="Downloaded PDF file path" sheetId="5" r:id="rId3"/>
-    <sheet name="Send Questionnaire Email" sheetId="7" r:id="rId4"/>
+    <sheet name="Send Questionnaire Email" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -34,12 +33,6 @@
   </si>
   <si>
     <t>spatil</t>
-  </si>
-  <si>
-    <t>Path for downloaded pdf file</t>
-  </si>
-  <si>
-    <t>C:\\Users\\compu\\Downloads\\Property_Name_Draft_AAI_05_ESA_01022017.pdf</t>
   </si>
   <si>
     <t>Site ID which is having ADA and FHA checklist, communication records under Supporting Documentation</t>
@@ -115,9 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -136,8 +128,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,32 +450,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64" style="6" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="64" style="5" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>7</v>
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1413725</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1413680</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -491,32 +487,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -526,68 +522,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>